<commit_message>
commit the flip implementation cause it's cool
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098E0B3B-A0AE-40CA-8045-F68B5F54D10F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3804CFEC-F7DA-47F4-A1BA-650F1983FB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9420" yWindow="5205" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.00000%"/>
+    <numFmt numFmtId="164" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -105,7 +105,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +424,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,13 +462,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>965376122</v>
+        <v>692746622</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>965376122</v>
+        <v>692746622</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -477,14 +477,14 @@
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>1050973</v>
+        <v>273680473</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>1050973</v>
+        <v>273680473</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -493,14 +493,14 @@
       </c>
       <c r="C5" s="1">
         <f>C4/C2</f>
-        <v>1.0874829621783317E-3</v>
+        <v>0.28318791393157289</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>1.0874829621783317E-3</v>
+        <v>0.28318791393157289</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FIRST PLACE AGAIN WOOO IT'S 4:45 AMMM
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F4BFBD-2B93-4B76-B303-92EF18DF7971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B88E631-4427-4935-9152-C6CE999145F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>139774710</v>
+        <v>3402436</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -467,13 +467,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>77969767</v>
+        <v>3402436</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3">
-        <v>77969767</v>
+        <v>3115976</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -482,14 +482,14 @@
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>888457328</v>
+        <v>963024659</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>61804943</v>
+        <v>286460</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -498,14 +498,14 @@
       </c>
       <c r="C5" s="1">
         <f>C4/C2</f>
-        <v>0.91932162560073916</v>
+        <v>0.99647936609227616</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>0.44217543359596312</v>
+        <v>8.4192619640751504E-2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>240717258</v>
+        <v>12121765</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
       </c>
       <c r="C11">
         <f>C9-C10</f>
-        <v>284051483</v>
+        <v>512646976</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -544,7 +544,7 @@
       </c>
       <c r="C12" s="1">
         <f>C11/C9</f>
-        <v>0.54128887795166902</v>
+        <v>0.97690074874334021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pipelining is a massive L
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2D55EF-D99A-40EB-B2B3-215770D06220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AB9BE2-3728-41E9-B229-51DD7DEC598C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -69,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +80,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,10 +113,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,6 +134,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>182120</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1DA375-4428-B96C-74D3-59B49F80A340}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3861955" y="1714500"/>
+          <a:ext cx="4286529" cy="3654136"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BF0C88-5804-4B96-BE0D-A9B40F600940}">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>3115976</v>
+        <v>2490772</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -467,13 +524,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>3402436</v>
+        <v>2490772</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3">
-        <v>2520532</v>
+        <v>2490772</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -482,14 +539,14 @@
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>963024659</v>
+        <v>963936323</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>595444</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -498,14 +555,14 @@
       </c>
       <c r="C5" s="1">
         <f>C4/C2</f>
-        <v>0.99647936609227616</v>
+        <v>0.99742270057111759</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>0.19109389802745591</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -518,15 +575,15 @@
         <v>1</v>
       </c>
       <c r="C9" s="2">
-        <v>524768741</v>
+        <v>12121765</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2">
-        <v>12121765</v>
+      <c r="C10" s="3">
+        <v>8738899</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -535,7 +592,7 @@
       </c>
       <c r="C11">
         <f>C9-C10</f>
-        <v>512646976</v>
+        <v>3382866</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -544,11 +601,12 @@
       </c>
       <c r="C12" s="1">
         <f>C11/C9</f>
-        <v>0.97690074874334021</v>
+        <v>0.27907371575014034</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
only log if needed. 9% speed improvement from last time
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2D55EF-D99A-40EB-B2B3-215770D06220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB19795-9C1C-404D-B2E4-7689CD6385B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -69,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +80,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,10 +113,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,6 +134,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>182120</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1DA375-4428-B96C-74D3-59B49F80A340}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3861955" y="1714500"/>
+          <a:ext cx="4286529" cy="3654136"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>352844</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>134299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DFEAF2C-6DDE-D3A2-751D-46929F30CE13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2476500"/>
+          <a:ext cx="3000794" cy="6801799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BF0C88-5804-4B96-BE0D-A9B40F600940}">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>3115976</v>
+        <v>2316182</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -467,13 +568,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>3402436</v>
+        <v>2460772</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3">
-        <v>2520532</v>
+        <v>2315900</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -482,14 +583,14 @@
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>963024659</v>
+        <v>963966323</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>595444</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -498,14 +599,14 @@
       </c>
       <c r="C5" s="1">
         <f>C4/C2</f>
-        <v>0.99647936609227616</v>
+        <v>0.99745374274714427</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>0.19109389802745591</v>
+        <v>1.2175209029342254E-4</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -518,15 +619,15 @@
         <v>1</v>
       </c>
       <c r="C9" s="2">
-        <v>524768741</v>
+        <v>12121765</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2">
-        <v>12121765</v>
+      <c r="C10" s="3">
+        <v>8738899</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -535,7 +636,7 @@
       </c>
       <c r="C11">
         <f>C9-C10</f>
-        <v>512646976</v>
+        <v>3382866</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -544,11 +645,12 @@
       </c>
       <c r="C12" s="1">
         <f>C11/C9</f>
-        <v>0.97690074874334021</v>
+        <v>0.27907371575014034</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
even more caching so faster
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A2B04B-39D5-46BC-ABD6-B950EF2F29D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F8AC79-3D01-4773-B99D-2FACDD0B3307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -479,7 +479,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1965372</v>
+        <v>1791425</v>
       </c>
       <c r="H2" s="3">
         <v>7828121</v>
@@ -490,13 +490,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>2287100</v>
+        <v>1801019</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3">
-        <v>1966620</v>
+        <v>1744385</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
@@ -508,14 +508,14 @@
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>964139995</v>
+        <v>964626076</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>-1248</v>
+        <v>47040</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -524,14 +524,14 @@
       </c>
       <c r="C5" s="1">
         <f>C4/C2</f>
-        <v>0.99763344797364151</v>
+        <v>0.99813641503914996</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>-6.3499429115709393E-4</v>
+        <v>2.625842555507487E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
i have ideas but i'm lazy
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF96C532-E630-4291-A9D3-91D880E569D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44DD1B4-1206-4748-94BE-15820297AAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -62,7 +62,7 @@
     <t>Test</t>
   </si>
   <si>
-    <t>https://miniodis-rproxy.lisn.upsaclay.fr/coda-v2-prod-private/detailed_result/2023-05-04-1683183569/74fa49e06405/detailed_results.html?AWSAccessKeyId=EASNOMJFX9QFW4QIY4SL&amp;Signature=vF7UKAb3bBCf%2FReClFuYHXYgvX8%3D&amp;Expires=1683269982#scores</t>
+    <t>results</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +492,7 @@
         <v>1738385</v>
       </c>
       <c r="H2" s="3">
-        <v>5823980</v>
+        <v>5813768</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" location="scores" xr:uid="{33B252D4-F0C2-4057-8FD8-E61B3BDFBCC9}"/>
+    <hyperlink ref="H3" r:id="rId1" location="result-for-submission" xr:uid="{33B252D4-F0C2-4057-8FD8-E61B3BDFBCC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
start reversing fft algo to use DIF FFT
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44DD1B4-1206-4748-94BE-15820297AAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B176FF6F-06B9-4ABC-92C9-35D51BF4A456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -102,11 +102,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF24292E"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color rgb="FF2C3F4C"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,13 +129,12 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -457,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +488,7 @@
       <c r="F2">
         <v>1738385</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>5813768</v>
       </c>
     </row>
@@ -508,7 +505,7 @@
       <c r="F3">
         <v>1728173</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -549,20 +546,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2">
-        <v>12121765</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="4">
+        <v>7685482</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="4">
-        <v>7828121</v>
+      <c r="C10" s="2">
+        <v>5813768</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -571,7 +568,7 @@
       </c>
       <c r="C11">
         <f>C9-C10</f>
-        <v>4293644</v>
+        <v>1871714</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -580,7 +577,7 @@
       </c>
       <c r="C12" s="1">
         <f>C11/C9</f>
-        <v>0.35420947362038446</v>
+        <v>0.24353892182689388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BACK WHERE WE BELONG
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B176FF6F-06B9-4ABC-92C9-35D51BF4A456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE0D168-FF50-4A62-A39F-E0232317319D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="F3">
-        <v>1728173</v>
+        <v>1522529</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>10212</v>
+        <v>215856</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>5.8744179223819814E-3</v>
+        <v>0.12417042254736436</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
i forgot you can just subtract like a normal person
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3188217E-D276-4667-A1D4-4A335F4D0E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A0D707-787B-4353-B122-2380B0969001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1738385</v>
+        <v>1522529</v>
       </c>
       <c r="H2" s="2">
         <v>5177717</v>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="F3">
-        <v>1522529</v>
+        <v>1338209</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>215856</v>
+        <v>184320</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>0.12417042254736436</v>
+        <v>0.12106173347108659</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
VECTORIZE THE BLACKMAN COEFS
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A0D707-787B-4353-B122-2380B0969001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD66871F-CBAF-4512-86FD-78008C4B0817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="180" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
+    <workbookView xWindow="18765" yWindow="5535" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF2C3F4C"/>
+      <color theme="1"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1522529</v>
+        <v>995739</v>
       </c>
       <c r="H2" s="2">
         <v>5177717</v>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="F3">
-        <v>1338209</v>
+        <v>992667</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>184320</v>
+        <v>3072</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>0.12106173347108659</v>
+        <v>3.0851458062805615E-3</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -546,20 +546,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4">
-        <v>7685482</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="C9" s="2">
+        <v>5813768</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2">
-        <v>5813768</v>
+      <c r="C10" s="4">
+        <v>4495733</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
       </c>
       <c r="C11">
         <f>C9-C10</f>
-        <v>1871714</v>
+        <v>1318035</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -577,7 +577,7 @@
       </c>
       <c r="C12" s="1">
         <f>C11/C9</f>
-        <v>0.24353892182689388</v>
+        <v>0.22670925293200556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get rid of useless math
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD66871F-CBAF-4512-86FD-78008C4B0817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99409308-1968-466F-B327-A66F631842C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18765" yWindow="5535" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,13 +497,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1522529</v>
+        <v>995739</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3">
-        <v>992667</v>
+        <v>954859</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
@@ -515,14 +515,14 @@
       </c>
       <c r="C4">
         <f>C2-C3</f>
-        <v>964904566</v>
+        <v>965431356</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>3072</v>
+        <v>40880</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -531,14 +531,14 @@
       </c>
       <c r="C5" s="1">
         <f>C4/C2</f>
-        <v>0.99842457955920616</v>
+        <v>0.99896966982284374</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>3.0851458062805615E-3</v>
+        <v>4.105493507836893E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MORE USELESS MATH GONE
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99409308-1968-466F-B327-A66F631842C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8859D185-F305-4EC6-9FE6-DE50719469E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18765" yWindow="5535" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F13" activeCellId="1" sqref="F3 F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="F3">
-        <v>954859</v>
+        <v>945169</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>40880</v>
+        <v>50570</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>4.105493507836893E-2</v>
+        <v>5.0786400854039057E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
what type of idiot thought moving buffers were a good idea
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60748B68-FBAB-4CB9-A54C-1E565339B86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C834F508-0176-43F5-B7BE-91E4A42D7112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18765" yWindow="5535" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
+    <workbookView xWindow="16005" yWindow="5100" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="F3">
-        <v>945169</v>
+        <v>929705</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>0</v>
+        <v>15464</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>0</v>
+        <v>1.6361095211544181E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
get ready to make it adjustable
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C834F508-0176-43F5-B7BE-91E4A42D7112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A2E199-0848-49A9-A3B9-A37B198711DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16005" yWindow="5100" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>945169</v>
+        <v>929705</v>
       </c>
       <c r="H2" s="2">
         <v>5177717</v>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="F3">
-        <v>929705</v>
+        <v>912245</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>15464</v>
+        <v>17460</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>1.6361095211544181E-2</v>
+        <v>1.8780150692961746E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
i love this piping architecture <3
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415FCAB0-A658-46F3-B522-BA3B3403F9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A80AF9B-AC06-4BAC-9992-AFB24F16EA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16005" yWindow="5100" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>682670</v>
+        <v>680380</v>
       </c>
       <c r="H2" s="2">
         <v>5177717</v>
@@ -502,9 +502,6 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3">
-        <v>671240</v>
-      </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
@@ -522,7 +519,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>11430</v>
+        <v>680380</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -538,7 +535,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>1.6743082309168413E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cleanup before optimization we are under a mili
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A80AF9B-AC06-4BAC-9992-AFB24F16EA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23E3CA5-0E54-475D-BAF7-BD90206E8A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16005" yWindow="5100" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +502,9 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
+      <c r="F3">
+        <v>523287</v>
+      </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
@@ -519,7 +522,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>680380</v>
+        <v>157093</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -535,7 +538,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>1</v>
+        <v>0.23089009083159412</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
last push before new yorkr
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnmal\source\repos\qualifiying_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23E3CA5-0E54-475D-BAF7-BD90206E8A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2857A2BB-8D23-4242-8F3A-C0705B494DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16005" yWindow="5100" windowWidth="18480" windowHeight="15345" xr2:uid="{91143030-D552-4C11-9E5F-8F8A1764BFAB}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>680380</v>
+        <v>261178</v>
       </c>
       <c r="H2" s="2">
         <v>5177717</v>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="F3">
-        <v>523287</v>
+        <v>261178</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="F4">
         <f>F2-F3</f>
-        <v>157093</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
       </c>
       <c r="F5" s="1">
         <f>F4/F2</f>
-        <v>0.23089009083159412</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>